<commit_message>
working on excel front end
</commit_message>
<xml_diff>
--- a/excel/Experimental.xlsx
+++ b/excel/Experimental.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\Documents\REPOS\capsim-12.4\excel frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\Documents\REPOS\capsim-12.4\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8CB7C2-3167-4E57-8F75-6D519D83519D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5FF250-AF9E-465D-8455-603B84253ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Title" sheetId="3" r:id="rId1"/>
+    <sheet name="Sources" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>https://www.scrapingbee.com/blog/how-to-send-post-python-requests/</t>
   </si>
@@ -43,16 +44,60 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=4dJ2vobI-G8</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/en-us/powerquery-m/m-spec-introduction</t>
+  </si>
+  <si>
+    <t>M language</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>capitalism.xlsx</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Alan Freeman</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>alan.freeman@umanitoba.ca</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Data source</t>
+  </si>
+  <si>
+    <t>Currently using downloaded json files; intention is to get from the active simulation on the website</t>
+  </si>
+  <si>
+    <t>Worbebnch to experiment on front end code for the capital simulation at datapaedia.org</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +120,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -359,43 +407,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D581D30A-5D7D-4322-85C7-40C1E0249394}">
+  <dimension ref="B2:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.15234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{206A48E6-5EE8-4DA0-8028-EB409F3593B6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="F2:G7"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="6:7" x14ac:dyDescent="0.4">
-      <c r="F2" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="6:7" x14ac:dyDescent="0.4">
-      <c r="G3" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="6:7" x14ac:dyDescent="0.4">
-      <c r="G4" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="6:7" x14ac:dyDescent="0.4">
-      <c r="G5" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="6:7" x14ac:dyDescent="0.4">
-      <c r="G6" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.4">
-      <c r="G7" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C7" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>